<commit_message>
Most country names aligned
</commit_message>
<xml_diff>
--- a/dat/WHORegions/WHORegions.xlsx
+++ b/dat/WHORegions/WHORegions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipsb/Dropbox/Projects/nCovForecast/dat/WHORegions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0461D43D-387D-C644-B7AB-DF25102CA735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B346799-5CA9-8E44-B0C2-3202BDCEFB8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54320" yWindow="-2600" windowWidth="10000" windowHeight="17040" xr2:uid="{044334A0-4D81-2045-8A04-599AED634F2B}"/>
+    <workbookView xWindow="39520" yWindow="-1940" windowWidth="10000" windowHeight="17040" xr2:uid="{044334A0-4D81-2045-8A04-599AED634F2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="206">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Angola</t>
   </si>
   <si>
-    <t>Antigua And Barbuda</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>Brunei Darussalam</t>
-  </si>
-  <si>
     <t>Bulgaria</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>Cape Verde</t>
-  </si>
-  <si>
     <t>Central African Republic</t>
   </si>
   <si>
@@ -149,18 +140,12 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>Congo</t>
-  </si>
-  <si>
     <t>Cook Islands</t>
   </si>
   <si>
     <t>Costa Rica</t>
   </si>
   <si>
-    <t>Côte d'Ivoire</t>
-  </si>
-  <si>
     <t>Croatia</t>
   </si>
   <si>
@@ -170,12 +155,6 @@
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Democratic Peoples Republic of Korea</t>
-  </si>
-  <si>
     <t>Democratic Republic of the Congo</t>
   </si>
   <si>
@@ -272,9 +251,6 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Iran, Islamic Republic of</t>
-  </si>
-  <si>
     <t>Iraq</t>
   </si>
   <si>
@@ -314,9 +290,6 @@
     <t>Kyrgyzstan</t>
   </si>
   <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
     <t>Latvia</t>
   </si>
   <si>
@@ -338,9 +311,6 @@
     <t>Luxembourg</t>
   </si>
   <si>
-    <t>Macedonia, the former Yugoslav Republic of</t>
-  </si>
-  <si>
     <t>Madagascar</t>
   </si>
   <si>
@@ -374,9 +344,6 @@
     <t>Micronesia, Federated States of</t>
   </si>
   <si>
-    <t>Moldova, Republic of</t>
-  </si>
-  <si>
     <t>Monaco</t>
   </si>
   <si>
@@ -392,9 +359,6 @@
     <t>Mozambique</t>
   </si>
   <si>
-    <t>Myanmar</t>
-  </si>
-  <si>
     <t>Namibia</t>
   </si>
   <si>
@@ -461,9 +425,6 @@
     <t>Romania</t>
   </si>
   <si>
-    <t>Russian Federation</t>
-  </si>
-  <si>
     <t>Rwanda</t>
   </si>
   <si>
@@ -482,9 +443,6 @@
     <t>San Marino</t>
   </si>
   <si>
-    <t>Sao Tome And Principe</t>
-  </si>
-  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
@@ -542,12 +500,6 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t>Tanzania, United Republic of</t>
-  </si>
-  <si>
     <t>Tajikistan</t>
   </si>
   <si>
@@ -590,9 +542,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>United States of America</t>
-  </si>
-  <si>
     <t>Uruguay</t>
   </si>
   <si>
@@ -605,9 +554,6 @@
     <t>Venezuela</t>
   </si>
   <si>
-    <t>Viet Nam</t>
-  </si>
-  <si>
     <t>Yemen</t>
   </si>
   <si>
@@ -642,6 +588,69 @@
   </si>
   <si>
     <t>WHO.Region</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Burma</t>
+  </si>
+  <si>
+    <t>Congo (Kinshasa)</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Korea, South</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Congo (Brazzaville)</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Taiwan*</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
   </si>
 </sst>
 </file>
@@ -993,23 +1002,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80F74A3-BBEA-DB4F-B627-3A20CF247BDC}">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1040,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,7 +1062,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,2080 +1073,2113 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>191</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>199</v>
       </c>
       <c r="B26">
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37">
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>200</v>
       </c>
       <c r="B41">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>193</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>194</v>
       </c>
       <c r="B50">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B51">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B55">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B59">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B61">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B62">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B69">
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B75">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B76">
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B77">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B78">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B79">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B80">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B81">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B82">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="B83">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B84">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B85">
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B87">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B88">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B89">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B91">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B92">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B95">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>189</v>
       </c>
       <c r="B97">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B98">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C99" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B100">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B101">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B102">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B103">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>195</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B106">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B107">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C108" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B109">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B110">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C112" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B114">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B116">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C116" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>202</v>
       </c>
       <c r="B117">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>103</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B119">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C119" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>118</v>
-      </c>
-      <c r="B120">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="C120" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B122">
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
       <c r="B123">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B124">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B125">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C125" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B126">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B127">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C128" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B130">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B131">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B132">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C132" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B133">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B134">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B135">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C135" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B136">
         <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B137">
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B139">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B140">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B141">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C141" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B142">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C142" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B143">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B144">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B145">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B146">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B147">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C147" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B148">
         <v>4</v>
       </c>
       <c r="C148" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B150">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C150" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C151" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B152">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="B153">
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>136</v>
+      </c>
+      <c r="B154">
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B155">
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>154</v>
-      </c>
-      <c r="B156">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="C156" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B157">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B158">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B159">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C159" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B161">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B162">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B163">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C163" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B164">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C164" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B165">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C166" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="B167">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B168">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B169">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B170">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C170" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B171">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B172">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C172" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="B173">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B174">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C174" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B175">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C175" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C176" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B177">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C177" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B178">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="B179">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C179" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B180">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C180" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B181">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="B182">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C182" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B183">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C183" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="B184">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C184" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B185">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C185" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B186">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C186" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B187">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B188">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B189">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C189" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B190">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C190" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B191">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C191" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B192">
         <v>14</v>
       </c>
       <c r="C192" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="B193">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C193" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B194">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C194" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B195">
+        <v>7</v>
+      </c>
+      <c r="C195" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>174</v>
+      </c>
+      <c r="B196">
         <v>2</v>
       </c>
-      <c r="C195" t="s">
-        <v>196</v>
+      <c r="C196" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>175</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>